<commit_message>
Update scheme excel file
</commit_message>
<xml_diff>
--- a/CampyCPS/db/CPS_scheme.xlsx
+++ b/CampyCPS/db/CPS_scheme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cui\Downloads\Campylobacter_CPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuiqingpo/Nutstore Files/Scripts/Python_Scripts/CampyCPS/CampyCPS/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C33B5C67-750F-4824-AF6F-4C448B53EAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E96505-A49C-8E42-A3EE-5634939A416E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{024147F8-3400-48BE-B366-3E56E0E6B168}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{024147F8-3400-48BE-B366-3E56E0E6B168}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t>Loci</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -350,6 +349,24 @@
   <si>
     <t>Gene/Aliases</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAMP1325</t>
+  </si>
+  <si>
+    <t>kpsC</t>
+  </si>
+  <si>
+    <t>Capsule polysaccharide modification protein (K07266)</t>
+  </si>
+  <si>
+    <t>CAMP1324</t>
+  </si>
+  <si>
+    <t>kpsS</t>
+  </si>
+  <si>
+    <t>Capsule polysaccharide modification protein (K07265)</t>
   </si>
 </sst>
 </file>
@@ -360,14 +377,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -427,7 +444,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -438,7 +455,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -770,21 +787,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378A8F57-1CA6-481E-95C0-7ED4A4C31CB0}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -795,7 +812,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -806,221 +823,221 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>74</v>
@@ -1028,65 +1045,65 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>74</v>
@@ -1094,21 +1111,21 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>74</v>
@@ -1116,56 +1133,78 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>